<commit_message>
Add implied "1" quantities
</commit_message>
<xml_diff>
--- a/SmartMatrixPhotonApa_bom.xlsx
+++ b/SmartMatrixPhotonApa_bom.xlsx
@@ -556,7 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -603,6 +605,9 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="D2" t="s">
         <v>45</v>
       </c>
@@ -617,6 +622,9 @@
       <c r="B3" t="s">
         <v>48</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3" t="s">
         <v>45</v>
       </c>
@@ -631,6 +639,9 @@
       <c r="B4" t="s">
         <v>20</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
       <c r="D4" t="s">
         <v>45</v>
       </c>
@@ -651,6 +662,9 @@
       <c r="B5" t="s">
         <v>46</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="D5" t="s">
         <v>45</v>
       </c>
@@ -688,6 +702,9 @@
       <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
       <c r="D7" t="s">
         <v>45</v>
       </c>
@@ -707,6 +724,9 @@
       </c>
       <c r="B8" t="s">
         <v>19</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Changes for V1 - Larger holes for APA102 wires - a 1x2 SMT jumper on bottom side of board for VIN and VEXT - optional (DNP) 6.3V 100uF smd 1206 cap to shield to help with USB power kickback when long strip switches - fatter VIN/VEXT to support USB power - photon dual header footprint improvements 	- Make it two parts as the connectors are two separate 2x12 headers 	- Fix the unnecessary DRC errors that show up in Eagle - change to shorter 2x12 connectors - update BOM - label pins used for microSD and apa - Put name on bottom of board (top is covered with Photon)
</commit_message>
<xml_diff>
--- a/SmartMatrixPhotonApa_bom.xlsx
+++ b/SmartMatrixPhotonApa_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="18940" windowHeight="17500" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="19160" windowHeight="21100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$29</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>RefDes</t>
   </si>
@@ -35,173 +38,170 @@
     <t>Name</t>
   </si>
   <si>
+    <t>RoHS</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Part#</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 10V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>microSD Socket</t>
+  </si>
+  <si>
+    <t>(optional) 4-pin terminal block</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>0 OHM 0603</t>
+  </si>
+  <si>
+    <t>47K 0603</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>2x12 SMT 0.1" Socket</t>
+  </si>
+  <si>
+    <t>MBR0520LT3GOSCT-ND</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 500MA SOD123</t>
+  </si>
+  <si>
+    <t>ON Semi</t>
+  </si>
+  <si>
+    <t>MBR0520LT3G</t>
+  </si>
+  <si>
+    <t>Alt Source</t>
+  </si>
+  <si>
+    <t>101-00660-68-6-1-ND</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>101-00660-68-6</t>
+  </si>
+  <si>
+    <t>4UCon 15882 - https://www.sparkfun.com/products/127</t>
+  </si>
+  <si>
+    <t>SN74AHCT1G08 SOT-23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-1113-1-ND </t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>SN74AHCT1G08DBVR</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 47K OHM 1% 1/10W 0603 </t>
+  </si>
+  <si>
+    <t>490-10517-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V 10% X7R 0805</t>
+  </si>
+  <si>
+    <t>399-1095-1-ND</t>
+  </si>
+  <si>
+    <t>KF120-4P</t>
+  </si>
+  <si>
+    <t>Kaweei</t>
+  </si>
+  <si>
+    <t>1276-5102-1-ND</t>
+  </si>
+  <si>
+    <t>4UCon 20087 - https://www.adafruit.com/products/2137</t>
+  </si>
+  <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>RoHS</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Part#</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 10V 10% X7R 0603</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>IC2, IC3</t>
-  </si>
-  <si>
-    <t>JP8</t>
-  </si>
-  <si>
-    <t>JP6</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>microSD Socket</t>
-  </si>
-  <si>
-    <t>(optional) 4-pin terminal block</t>
-  </si>
-  <si>
-    <t>DNP</t>
-  </si>
-  <si>
-    <t>0 OHM 0603</t>
-  </si>
-  <si>
-    <t>47K 0603</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>DIODE SCHOTTKY 60V 500MA SOD123</t>
-  </si>
-  <si>
-    <t>JP2, JP3</t>
-  </si>
-  <si>
-    <t>2x12 SMT 0.1" Socket</t>
-  </si>
-  <si>
-    <t>MBR0520LT3GOSCT-ND</t>
-  </si>
-  <si>
-    <t>DIODE SCHOTTKY 20V 500MA SOD123</t>
-  </si>
-  <si>
-    <t>ON Semi</t>
-  </si>
-  <si>
-    <t>MBR0520LT3G</t>
-  </si>
-  <si>
-    <t>Alt Source</t>
-  </si>
-  <si>
-    <t>101-00660-68-6-1-ND</t>
-  </si>
-  <si>
-    <t>Amphenol</t>
-  </si>
-  <si>
-    <t>101-00660-68-6</t>
-  </si>
-  <si>
-    <t>4UCon 15882 - https://www.sparkfun.com/products/127</t>
-  </si>
-  <si>
-    <t>3M9577CT-ND</t>
-  </si>
-  <si>
-    <t>3M</t>
-  </si>
-  <si>
-    <t>966224-2000-AR-PR</t>
-  </si>
-  <si>
-    <t>SN74AHCT1G08 SOT-23-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-1113-1-ND </t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>SN74AHCT1G08DBVR</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 47K OHM 1% 1/10W 0603 </t>
-  </si>
-  <si>
-    <t>490-10517-1-ND</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 10V 10% X7R 0805</t>
-  </si>
-  <si>
-    <t>399-1095-1-ND</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/products/2137</t>
-  </si>
-  <si>
-    <t>KF120-4P</t>
-  </si>
-  <si>
-    <t>Kaweei</t>
-  </si>
-  <si>
-    <t>1276-5102-1-ND</t>
-  </si>
-  <si>
-    <t>Solder Jumper</t>
-  </si>
-  <si>
-    <t>4UCon 13111? (too short?), China source TBD</t>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>1x2 SMT 0.1" pins</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>CAP CER 100UF 6.3V X5R</t>
+  </si>
+  <si>
+    <t>4UCon</t>
+  </si>
+  <si>
+    <t>Samtec SSM-112-F-DV-BE</t>
+  </si>
+  <si>
+    <t>Samtec TSM-102-01-T-SH</t>
+  </si>
+  <si>
+    <t>JP3,JP4</t>
+  </si>
+  <si>
+    <t>IC1, IC2</t>
+  </si>
+  <si>
+    <t>Any</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -225,6 +225,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -243,7 +249,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -258,14 +264,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="50">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -276,9 +321,45 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,18 +635,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -577,246 +660,256 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>45</v>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>45</v>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>45</v>
+      <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>32</v>
+      <c r="I7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" t="s">
-        <v>37</v>
+        <v>49</v>
+      </c>
+      <c r="H8" s="1">
+        <v>13111</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="H9" s="1">
+        <v>13402</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="63" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>